<commit_message>
AutoCommit_11 июля 2024 г. 15:22:27_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322/2ОИБАС1322_УП_.xlsx
+++ b/2ОИБАС1322/2ОИБАС1322_УП_.xlsx
@@ -549,7 +549,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -717,6 +717,12 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
       <c r="M7" s="3"/>
       <c r="N7" s="2"/>
       <c r="S7" s="6"/>
@@ -1066,6 +1072,9 @@
       <c r="D24" s="2"/>
       <c r="E24" s="3"/>
       <c r="F24" s="4"/>
+      <c r="G24">
+        <v>5</v>
+      </c>
       <c r="I24" s="4"/>
       <c r="M24" s="3"/>
       <c r="N24" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_11 июля 2024 г. 15:27:03_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1322/2ОИБАС1322_УП_.xlsx
+++ b/2ОИБАС1322/2ОИБАС1322_УП_.xlsx
@@ -549,7 +549,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -629,8 +629,12 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="F3" s="4">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4">
+        <v>5</v>
+      </c>
       <c r="I3" s="4"/>
       <c r="J3" s="9"/>
       <c r="M3" s="3"/>
@@ -716,7 +720,18 @@
         <v>4</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
       <c r="I7">
         <v>5</v>
       </c>
@@ -801,8 +816,21 @@
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="2"/>
+      <c r="D11" s="3">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
       <c r="J11">
         <v>5</v>
       </c>
@@ -822,8 +850,12 @@
         <v>9</v>
       </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
+      <c r="E12" s="3">
+        <v>5</v>
+      </c>
+      <c r="F12" s="4">
+        <v>5</v>
+      </c>
       <c r="G12" s="4"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
@@ -1032,6 +1064,15 @@
         <v>5</v>
       </c>
       <c r="E22" s="2">
+        <v>5</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="H22">
         <v>5</v>
       </c>
       <c r="J22">
@@ -1118,8 +1159,12 @@
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="F26" s="4">
+        <v>5</v>
+      </c>
+      <c r="G26" s="4">
+        <v>5</v>
+      </c>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>

</xml_diff>